<commit_message>
Added more TC for register webpage
</commit_message>
<xml_diff>
--- a/UDEMY_Selenium_with_Python/Pytest_Selenium_Framework/test_data/Opencart_LoginData.xlsx
+++ b/UDEMY_Selenium_with_Python/Pytest_Selenium_Framework/test_data/Opencart_LoginData.xlsx
@@ -8,7 +8,7 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Registration" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="124519"/>
   <extLst>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="15">
   <si>
     <t>username</t>
   </si>
@@ -58,23 +58,20 @@
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t xml:space="preserve"> username</t>
-  </si>
-  <si>
-    <t>Uesrname</t>
-  </si>
-  <si>
-    <t xml:space="preserve">username </t>
-  </si>
-  <si>
-    <t>user name</t>
+    <t>email</t>
+  </si>
+  <si>
+    <t>johndoe.example.com</t>
+  </si>
+  <si>
+    <t>johndoe@example</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -94,14 +91,6 @@
       <b/>
       <sz val="14"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="12"/>
-      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -161,19 +150,19 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -494,15 +483,15 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A7"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="30.33203125" style="5" customWidth="1"/>
-    <col min="2" max="2" width="25.109375" style="5" customWidth="1"/>
-    <col min="3" max="3" width="22" style="5" customWidth="1"/>
-    <col min="4" max="16384" width="8.88671875" style="5"/>
+    <col min="1" max="1" width="30.33203125" style="4" customWidth="1"/>
+    <col min="2" max="2" width="25.109375" style="4" customWidth="1"/>
+    <col min="3" max="3" width="22" style="4" customWidth="1"/>
+    <col min="4" max="16384" width="8.88671875" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="18" x14ac:dyDescent="0.35">
@@ -516,81 +505,75 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:3" s="4" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:3" s="3" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" s="4" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
+    <row r="3" spans="1:3" s="3" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:3" s="4" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
+    <row r="4" spans="1:3" s="3" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A4" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:3" s="4" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
+    <row r="5" spans="1:3" s="3" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A5" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:3" s="4" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A6" s="3" t="s">
+    <row r="6" spans="1:3" s="3" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="2" t="s">
         <v>3</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A5" r:id="rId1" display="pavan@gmail.com"/>
-    <hyperlink ref="A4" r:id="rId2" display="pavan@gmail.com"/>
-    <hyperlink ref="A3" r:id="rId3" display="pavanoltraining@gmail.com"/>
-    <hyperlink ref="A2" r:id="rId4" display="pavanoltraining@gmail.com"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId5"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -599,56 +582,61 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="31.21875" style="5" customWidth="1"/>
-    <col min="2" max="2" width="22" style="5" customWidth="1"/>
-    <col min="3" max="16384" width="8.88671875" style="5"/>
+    <col min="1" max="1" width="31.21875" style="4" customWidth="1"/>
+    <col min="2" max="2" width="30.21875" style="4" customWidth="1"/>
+    <col min="3" max="16384" width="8.88671875" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:2" s="4" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B2" s="3"/>
-    </row>
-    <row r="3" spans="1:2" s="4" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
+    <row r="2" spans="1:2" s="3" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" s="3" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A3" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="3"/>
-    </row>
-    <row r="4" spans="1:2" s="4" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A4" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B4" s="3"/>
-    </row>
-    <row r="5" spans="1:2" s="4" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3"/>
-    </row>
-    <row r="6" spans="1:2" s="4" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A6" s="3"/>
-      <c r="B6" s="3"/>
+      <c r="B3" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" s="3" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A4" s="2"/>
+      <c r="B4" s="2"/>
+    </row>
+    <row r="5" spans="1:2" s="3" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A5" s="2"/>
+      <c r="B5" s="2"/>
+    </row>
+    <row r="6" spans="1:2" s="3" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A6" s="2"/>
+      <c r="B6" s="2"/>
     </row>
     <row r="7" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A7" s="3"/>
-      <c r="B7" s="3"/>
+      <c r="A7" s="2"/>
+      <c r="B7" s="2"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A3" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>